<commit_message>
adding tableau food bank geo map and R correlation in Power BI
</commit_message>
<xml_diff>
--- a/Timeline_ template.xlsx
+++ b/Timeline_ template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annru\Documents\capstone_annrumsey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8BD078-C970-484B-B35D-75FDE5DD0C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809E55C6-390A-4C96-84D4-C2A00BCC8605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3E5591EE-1479-4915-B308-C3BDB3157271}"/>
   </bookViews>
@@ -668,7 +668,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{654E463E-D664-4DE5-8995-2308488F4B10}" type="CELLRANGE">
+                    <a:fld id="{287F7C87-A511-4407-B73E-AA81C40A7527}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -702,7 +702,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6876E4C-EAD5-4C07-8E71-67C9D6380232}" type="CELLRANGE">
+                    <a:fld id="{9109558A-D857-47B7-BE5E-7F15C5D0CF6E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -736,7 +736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAB48597-9F45-4D52-984B-536C1309E327}" type="CELLRANGE">
+                    <a:fld id="{E7AC3D07-0615-4069-9F9A-6F9D8DB56846}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -770,7 +770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A788095-8B55-4591-84A5-643623D71D31}" type="CELLRANGE">
+                    <a:fld id="{A3AA657C-C17B-437E-A30C-7A8DF55C6EEC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -804,7 +804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B86D1917-3EDF-4897-9C23-910E1139A403}" type="CELLRANGE">
+                    <a:fld id="{EFCD4ABF-B7F8-42A8-B2BA-BCD2422A38A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -838,7 +838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA5C1A16-5485-4F2B-ABCA-C8DF52622604}" type="CELLRANGE">
+                    <a:fld id="{905EA066-EFC9-4DBD-B268-6AF1F2C04457}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -872,7 +872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BEF7DB5-0A1D-45F0-B142-4223DDC10B02}" type="CELLRANGE">
+                    <a:fld id="{8719DA94-5B16-4B68-9B57-5623AA16E3D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -906,7 +906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E86A1073-ACF2-4315-B60D-40EB096185D3}" type="CELLRANGE">
+                    <a:fld id="{C56BC478-99A9-431D-ACE9-30C985FB66E2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -940,7 +940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{557C5FD0-9633-4767-9E50-14CCEC8777BA}" type="CELLRANGE">
+                    <a:fld id="{DE85BFC4-537E-45C0-9421-FB875E33489A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -974,7 +974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B5AAA24-FEE2-49AC-9AAA-EB0EE9F712AD}" type="CELLRANGE">
+                    <a:fld id="{60363C12-5DB9-4625-ABEB-6A67F8280239}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1008,7 +1008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DACA05F5-8326-4FD9-97D0-BDDD6D9FCA27}" type="CELLRANGE">
+                    <a:fld id="{8EA1E956-1F4B-4538-8F98-D48BE5ED6698}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1042,7 +1042,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE36CD8E-15F6-4441-8D1E-8AE385637623}" type="CELLRANGE">
+                    <a:fld id="{FD8C9E19-9DE9-4BAF-A082-C201FD23EF64}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1076,7 +1076,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98BD0B00-1789-4139-847B-CCA9BDF09B76}" type="CELLRANGE">
+                    <a:fld id="{CA8B1DB8-7237-476C-B23C-2721E9CF6F83}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1110,7 +1110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5007FF7A-8E17-4745-A82D-9339353DE772}" type="CELLRANGE">
+                    <a:fld id="{C5DC1F0C-E3DC-4B54-9DC8-DE04CCB45EA1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1144,7 +1144,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D9B0F1D-5879-413F-A528-878457A988F2}" type="CELLRANGE">
+                    <a:fld id="{120B2745-663C-4E8D-B422-6AEFACD0001F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1178,7 +1178,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E7A58A5-958D-47D8-B56A-F9A22B10A160}" type="CELLRANGE">
+                    <a:fld id="{3D56EFD3-2AEC-45CE-A156-49319BB28976}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1212,7 +1212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F26CE55-9D91-4CB7-B316-EA3EE889649A}" type="CELLRANGE">
+                    <a:fld id="{88862FEC-635B-4AE5-A040-8C6339D333FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1246,7 +1246,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D6F43DA-748D-4FFA-AEFD-17C4C0F2C36D}" type="CELLRANGE">
+                    <a:fld id="{D537F7A9-74D3-432E-9558-57FD6797858F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1280,7 +1280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93587765-4ECB-4060-9D93-5D82E606C95D}" type="CELLRANGE">
+                    <a:fld id="{014D0421-1240-4026-92BC-F432221D983E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1314,7 +1314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{04DCF0CD-8AED-47CA-B04E-EAB6BB54EC56}" type="CELLRANGE">
+                    <a:fld id="{4CC92FC7-19E3-4C76-978B-775BF20E3A51}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1348,7 +1348,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA7B6092-D81B-410D-BBE0-57C4921BE86D}" type="CELLRANGE">
+                    <a:fld id="{66F57B8C-C672-4EAF-9B19-D8B616BA08DA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1382,7 +1382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A9528A7-FA2D-45CB-9484-B3598E7F0336}" type="CELLRANGE">
+                    <a:fld id="{8F2F23E8-6FB0-4D49-A94F-4783CFE03610}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1416,7 +1416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8FCA8080-336A-42B7-8D31-0D49B17CA6ED}" type="CELLRANGE">
+                    <a:fld id="{6F714536-DC03-407F-B793-520A12DCEFDE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1450,7 +1450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7C66E77-3C3C-4284-A03D-2ACEBB3130FD}" type="CELLRANGE">
+                    <a:fld id="{097F6E5E-8596-4433-AA00-7F05D194B813}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1484,7 +1484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4242258F-01A3-45E7-BE0C-5DACDC60B5C4}" type="CELLRANGE">
+                    <a:fld id="{4009BBAF-4CEC-474C-BF88-645733AC3E4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1518,7 +1518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8C62D043-4ABE-40BC-9D1E-45F9F3964519}" type="CELLRANGE">
+                    <a:fld id="{73003112-21A0-4B66-BD9C-F19FABBFCB00}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1552,7 +1552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9AF76D4C-A95B-4F64-B16B-BBC929836EDF}" type="CELLRANGE">
+                    <a:fld id="{FC10374D-3081-461D-AD36-78934DE093B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1586,7 +1586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{246F1BB4-67D4-49E0-BC44-25878D996D09}" type="CELLRANGE">
+                    <a:fld id="{83388379-C4A2-42FC-B63A-2B50C19C99D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1620,7 +1620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2F42574-34E5-4836-8935-011AB9328936}" type="CELLRANGE">
+                    <a:fld id="{0D106FCE-3D92-4399-A363-E41586AAC387}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1654,7 +1654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8EE99B1-5E30-4070-8538-297A44C4587A}" type="CELLRANGE">
+                    <a:fld id="{3848C041-4902-4716-B19A-DA947C6714B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1688,7 +1688,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E6CC36A-315A-44BD-AF54-04C50BA7CC3D}" type="CELLRANGE">
+                    <a:fld id="{79EF6DEE-F528-43CC-9173-9E6B604BF683}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1722,7 +1722,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7189485-D1A4-4053-B4CB-CFDF61CA46B2}" type="CELLRANGE">
+                    <a:fld id="{4AF66706-D087-48CF-97EF-141B7A0F4A53}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1756,7 +1756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2457F5BF-8EB1-4E9B-8CCC-00D07B3AAD07}" type="CELLRANGE">
+                    <a:fld id="{38F724C8-5B61-44F8-8C06-4DAB2C0FCF5D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1790,7 +1790,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8683893-BC08-4FBB-9B59-C6C52A187716}" type="CELLRANGE">
+                    <a:fld id="{6CAAE838-019D-476D-A89E-EC818BA63EEA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1824,7 +1824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DEDF11C5-F505-4AE3-BF5D-61D20C6C8EEF}" type="CELLRANGE">
+                    <a:fld id="{CF6A89D9-EBAC-46B1-8683-5EA885878A0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1858,7 +1858,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2847F502-1CC0-468C-83F5-BC280F41632D}" type="CELLRANGE">
+                    <a:fld id="{9F3ABFF5-6AB5-4916-9C35-1DE1E721493C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1892,7 +1892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F63FA50A-C9FD-4BB2-A9F9-EC673A04E981}" type="CELLRANGE">
+                    <a:fld id="{A3B7F428-F4CA-4DCA-9130-BF40DDFF42B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1926,7 +1926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5029E62B-524C-4D86-923E-018F9F3B6FD7}" type="CELLRANGE">
+                    <a:fld id="{80F10AD1-D9CA-4091-8250-277DEE97DC99}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1960,7 +1960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A881DD70-B96B-4BC6-9C7F-180CAF6AD506}" type="CELLRANGE">
+                    <a:fld id="{FFFBAE12-3B2A-487A-B719-1AB0C08C35B8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1994,7 +1994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3CA34E1-AFB7-4E6E-87B6-23DE8EC0B3E8}" type="CELLRANGE">
+                    <a:fld id="{61525D00-619D-4309-B849-01C90977BA62}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2028,7 +2028,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEE57BE5-5075-4177-9CBB-D5D0C587D42C}" type="CELLRANGE">
+                    <a:fld id="{6E670091-9D32-462A-8C76-10F0B6DBB9D8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2062,7 +2062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{86D129FA-F2E3-42FC-9ED7-BAD7CA1FCE23}" type="CELLRANGE">
+                    <a:fld id="{CC1C0F58-133A-4294-BC91-7D0B0C32ADF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2096,7 +2096,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A7496D2-6BF9-4ABB-90B5-23052970CE19}" type="CELLRANGE">
+                    <a:fld id="{E709E05D-EBC3-4670-AB31-EE1A03E3DB7C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2130,7 +2130,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3D39F6C-D3B3-4A73-B4B6-F86D748D4E09}" type="CELLRANGE">
+                    <a:fld id="{AC691A59-308B-467C-A7CD-84E63058019C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2164,7 +2164,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{692BC66F-673F-44C5-B08F-FFE86C4D0ADC}" type="CELLRANGE">
+                    <a:fld id="{BF369BD2-6873-4105-A838-AF699220A457}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2198,7 +2198,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0A8DE46-CD21-4076-A7F2-79F7502C9BC2}" type="CELLRANGE">
+                    <a:fld id="{03474D1A-E819-48AD-A0DB-B989A8D9CC2B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2232,7 +2232,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03EA5833-AB3A-4695-A78D-5FAA4AE348B2}" type="CELLRANGE">
+                    <a:fld id="{DC8E5851-C4CF-4E6B-BA1C-D179235591F0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2266,7 +2266,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6BF1E8B-7DF3-4C90-A656-9DDBDC09FC38}" type="CELLRANGE">
+                    <a:fld id="{7AD1FC92-6FCB-47D9-B55A-C958D64BAC77}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2300,7 +2300,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{868C173D-651E-4EAA-8EF1-8A66CC0C9594}" type="CELLRANGE">
+                    <a:fld id="{FD57845B-F325-472E-8AFA-C9269631FD09}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2334,7 +2334,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A5051ED-B912-43C8-ACC4-E24EEC49344C}" type="CELLRANGE">
+                    <a:fld id="{DA388131-98F5-4387-B43F-4351B4806C81}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2368,7 +2368,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F68C2E9-9FA4-45F7-B4ED-4C795F9219F9}" type="CELLRANGE">
+                    <a:fld id="{787D555D-23BE-40CE-9203-9D09E9FE1E46}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2402,7 +2402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{331BF2CE-DF20-4FFD-9507-A73CE48DE352}" type="CELLRANGE">
+                    <a:fld id="{39EE4C14-1022-4521-B00A-3C48ECE35B1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2436,7 +2436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E91C8FE-4054-4F3A-9C41-99B0146D6009}" type="CELLRANGE">
+                    <a:fld id="{93239FB3-1B8F-4251-8395-B763DC1FCF31}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2470,7 +2470,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3892B347-6A09-4DB1-B43F-07157630FBDE}" type="CELLRANGE">
+                    <a:fld id="{BE500AF6-4F16-41DF-A5B8-7DE16159281D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2504,7 +2504,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F26B9A19-EE28-4ADA-B06C-358FF4FFC992}" type="CELLRANGE">
+                    <a:fld id="{AE16F8B6-75E2-4EF6-97D2-3AF6095B464F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2538,7 +2538,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD2C1FD1-54E3-45BA-B731-3668D930AFE0}" type="CELLRANGE">
+                    <a:fld id="{84BDC303-5A0B-4273-996D-D277B0C292A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2572,7 +2572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{188DB96E-263B-488B-AECA-6E79FDA0DB6F}" type="CELLRANGE">
+                    <a:fld id="{76C27FE7-78E7-480D-B40D-30C2FCA5B065}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2606,7 +2606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2DF39648-D40D-44EF-A888-4B4C805D3341}" type="CELLRANGE">
+                    <a:fld id="{89B6373F-F9BC-4D88-8EF9-3E3E91A57D0A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2640,7 +2640,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF45EC2C-C3C0-4B11-8A23-774D15D8010F}" type="CELLRANGE">
+                    <a:fld id="{CCABF0B1-7E02-42DF-B590-5A06CAB6C6D6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2674,7 +2674,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EE001DC-BC6C-4B9B-ADA6-1CF84C123928}" type="CELLRANGE">
+                    <a:fld id="{BAF18C23-B7DE-4507-B234-0899F212424C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3399,20 +3399,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3435,7 +3421,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3462,24 +3448,10 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3540,14 +3512,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="accent5">
+        <a:lumMod val="20000"/>
+        <a:lumOff val="80000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -4468,7 +4440,7 @@
   <dimension ref="A30:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T89" sqref="T89"/>
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
uploading shell of PowerPoint to start tracking
</commit_message>
<xml_diff>
--- a/Timeline_ template.xlsx
+++ b/Timeline_ template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annru\Documents\capstone_annrumsey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809E55C6-390A-4C96-84D4-C2A00BCC8605}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59F8151-50F4-437A-A16F-0E0899A91EA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3E5591EE-1479-4915-B308-C3BDB3157271}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{3E5591EE-1479-4915-B308-C3BDB3157271}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>Year</t>
   </si>
@@ -477,12 +477,18 @@
   <si>
     <t>2022 Bioengineered Food labels</t>
   </si>
+  <si>
+    <t>FDA Announces Plant and Animal Biotechnology Innovation Action Plan</t>
+  </si>
+  <si>
+    <t>FDA deactivation of an import alert on genetically engineered salmon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +555,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -571,7 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -597,6 +610,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -668,7 +682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{287F7C87-A511-4407-B73E-AA81C40A7527}" type="CELLRANGE">
+                    <a:fld id="{EEF157FB-4593-4D33-B6ED-6A0F2E9E4DFE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -702,7 +716,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9109558A-D857-47B7-BE5E-7F15C5D0CF6E}" type="CELLRANGE">
+                    <a:fld id="{6DABE872-DE0D-4CE7-A201-4352A46CBDDB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -736,7 +750,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7AC3D07-0615-4069-9F9A-6F9D8DB56846}" type="CELLRANGE">
+                    <a:fld id="{7215229C-AD75-4093-BC6E-E0629B7D3B41}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -770,7 +784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3AA657C-C17B-437E-A30C-7A8DF55C6EEC}" type="CELLRANGE">
+                    <a:fld id="{9C0060A9-1669-4B5E-A638-4B09F38EA961}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -804,7 +818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFCD4ABF-B7F8-42A8-B2BA-BCD2422A38A1}" type="CELLRANGE">
+                    <a:fld id="{4B789163-6573-4E20-A19E-B5EB965010DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -838,7 +852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{905EA066-EFC9-4DBD-B268-6AF1F2C04457}" type="CELLRANGE">
+                    <a:fld id="{19F98B79-E674-4880-9CB6-E193EA7CF634}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -872,7 +886,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8719DA94-5B16-4B68-9B57-5623AA16E3D1}" type="CELLRANGE">
+                    <a:fld id="{6029CA03-AEEC-43B6-B0E0-6C6A0BCDCED3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -906,7 +920,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C56BC478-99A9-431D-ACE9-30C985FB66E2}" type="CELLRANGE">
+                    <a:fld id="{6FD3CE55-F9E6-4939-AF3C-E183EF52083E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -940,7 +954,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE85BFC4-537E-45C0-9421-FB875E33489A}" type="CELLRANGE">
+                    <a:fld id="{28A9ECA4-E759-48CC-B190-C2A64BA775C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -974,7 +988,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{60363C12-5DB9-4625-ABEB-6A67F8280239}" type="CELLRANGE">
+                    <a:fld id="{DDAF7600-CD0D-47EA-A5F1-D9A134687532}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1008,7 +1022,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EA1E956-1F4B-4538-8F98-D48BE5ED6698}" type="CELLRANGE">
+                    <a:fld id="{7AAE52DF-D2BA-4840-A76E-1CAAF55B6AE2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1042,7 +1056,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD8C9E19-9DE9-4BAF-A082-C201FD23EF64}" type="CELLRANGE">
+                    <a:fld id="{3E35C1F1-85E1-4C7C-9A23-DFB13D4B6FC7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1076,7 +1090,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CA8B1DB8-7237-476C-B23C-2721E9CF6F83}" type="CELLRANGE">
+                    <a:fld id="{F8F641A8-6F5F-4F89-9C9B-B00C99D4CB97}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1110,7 +1124,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5DC1F0C-E3DC-4B54-9DC8-DE04CCB45EA1}" type="CELLRANGE">
+                    <a:fld id="{EB0A50A7-FCEA-4EAA-9BEA-DDDB135D23EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1144,7 +1158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{120B2745-663C-4E8D-B422-6AEFACD0001F}" type="CELLRANGE">
+                    <a:fld id="{F5F2F0FB-3A2A-42CA-B748-5DE339F55766}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1178,7 +1192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D56EFD3-2AEC-45CE-A156-49319BB28976}" type="CELLRANGE">
+                    <a:fld id="{5DA63A12-F687-4923-83AA-8054AB1DE90F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1212,7 +1226,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88862FEC-635B-4AE5-A040-8C6339D333FF}" type="CELLRANGE">
+                    <a:fld id="{0C24CD87-B3F2-48DC-B22C-F89A7962D5E4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1246,7 +1260,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D537F7A9-74D3-432E-9558-57FD6797858F}" type="CELLRANGE">
+                    <a:fld id="{C05EBD74-692F-4D62-A822-04CAB04AF405}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1280,7 +1294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{014D0421-1240-4026-92BC-F432221D983E}" type="CELLRANGE">
+                    <a:fld id="{224F08B4-9B88-4EC4-9764-C4863A58A99D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1314,7 +1328,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4CC92FC7-19E3-4C76-978B-775BF20E3A51}" type="CELLRANGE">
+                    <a:fld id="{FC8FBE75-4FA5-4380-A127-E3DAC4A09882}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1348,7 +1362,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66F57B8C-C672-4EAF-9B19-D8B616BA08DA}" type="CELLRANGE">
+                    <a:fld id="{570AC00F-4915-4A29-A5D7-C17C7A37B1D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1382,7 +1396,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F2F23E8-6FB0-4D49-A94F-4783CFE03610}" type="CELLRANGE">
+                    <a:fld id="{E507077B-1345-48D1-B6DD-7EAEA7EFE85D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1416,7 +1430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F714536-DC03-407F-B793-520A12DCEFDE}" type="CELLRANGE">
+                    <a:fld id="{2E5EF788-1097-4809-8A7F-F9EBF6B329CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1450,7 +1464,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{097F6E5E-8596-4433-AA00-7F05D194B813}" type="CELLRANGE">
+                    <a:fld id="{CD01CBB6-D322-417B-A5DB-F66C00FE01D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1484,7 +1498,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4009BBAF-4CEC-474C-BF88-645733AC3E4A}" type="CELLRANGE">
+                    <a:fld id="{554BFF2B-B9FB-467C-8C07-C8F56C147F18}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1518,7 +1532,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{73003112-21A0-4B66-BD9C-F19FABBFCB00}" type="CELLRANGE">
+                    <a:fld id="{BA89D949-05D9-4B34-88C4-A79A6E309949}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1552,7 +1566,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC10374D-3081-461D-AD36-78934DE093B0}" type="CELLRANGE">
+                    <a:fld id="{702843F7-A211-41FF-ACD3-7930FBC6202A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1586,7 +1600,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83388379-C4A2-42FC-B63A-2B50C19C99D8}" type="CELLRANGE">
+                    <a:fld id="{72EEDD67-5853-4368-879E-2051AA3A4C4D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1620,7 +1634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D106FCE-3D92-4399-A363-E41586AAC387}" type="CELLRANGE">
+                    <a:fld id="{CB26A554-78EB-412B-B5CB-E518F396DA57}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1654,7 +1668,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3848C041-4902-4716-B19A-DA947C6714B0}" type="CELLRANGE">
+                    <a:fld id="{457441B7-BEAF-497A-B5DD-C93C62E7E8C0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1688,7 +1702,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79EF6DEE-F528-43CC-9173-9E6B604BF683}" type="CELLRANGE">
+                    <a:fld id="{3258D22F-9576-47E7-ADDC-77F590CE5422}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1722,7 +1736,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AF66706-D087-48CF-97EF-141B7A0F4A53}" type="CELLRANGE">
+                    <a:fld id="{2399F71D-169F-4636-BBF9-8F1FE08937FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1756,7 +1770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38F724C8-5B61-44F8-8C06-4DAB2C0FCF5D}" type="CELLRANGE">
+                    <a:fld id="{423ECD27-115D-4CD7-BA5A-0C11682D5EA8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1790,7 +1804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CAAE838-019D-476D-A89E-EC818BA63EEA}" type="CELLRANGE">
+                    <a:fld id="{2B3B5C18-DC4F-4760-853D-FACE073F07AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1824,7 +1838,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF6A89D9-EBAC-46B1-8683-5EA885878A0E}" type="CELLRANGE">
+                    <a:fld id="{5304F656-8DC1-47D5-8D9B-C9343E5D21FD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1858,7 +1872,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F3ABFF5-6AB5-4916-9C35-1DE1E721493C}" type="CELLRANGE">
+                    <a:fld id="{874971DA-A155-4D3F-9EEE-EEA0DA7E9291}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1892,7 +1906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3B7F428-F4CA-4DCA-9130-BF40DDFF42B9}" type="CELLRANGE">
+                    <a:fld id="{13EDF590-DE9B-4C64-8109-3F5700EBFF5E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1926,7 +1940,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80F10AD1-D9CA-4091-8250-277DEE97DC99}" type="CELLRANGE">
+                    <a:fld id="{7C126BC2-0983-4DDF-A560-1F3A89AD07EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1960,7 +1974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FFFBAE12-3B2A-487A-B719-1AB0C08C35B8}" type="CELLRANGE">
+                    <a:fld id="{B6FE13CB-6347-44EC-A0F0-34F49303F5C6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1994,7 +2008,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61525D00-619D-4309-B849-01C90977BA62}" type="CELLRANGE">
+                    <a:fld id="{1B72B7B4-EED1-4293-ABE5-751562B422F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2028,7 +2042,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E670091-9D32-462A-8C76-10F0B6DBB9D8}" type="CELLRANGE">
+                    <a:fld id="{EB4130CB-1439-4A78-9821-3277D6FA6657}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2062,7 +2076,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC1C0F58-133A-4294-BC91-7D0B0C32ADF5}" type="CELLRANGE">
+                    <a:fld id="{B70977E5-E04F-4E93-8174-238705DE5A1A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2096,7 +2110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E709E05D-EBC3-4670-AB31-EE1A03E3DB7C}" type="CELLRANGE">
+                    <a:fld id="{354B5F78-A02C-4555-B489-8BE5C7E4BB9E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2130,7 +2144,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AC691A59-308B-467C-A7CD-84E63058019C}" type="CELLRANGE">
+                    <a:fld id="{5C62AAC3-E6E5-4DF8-A0DD-1891DC68AB85}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2164,7 +2178,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF369BD2-6873-4105-A838-AF699220A457}" type="CELLRANGE">
+                    <a:fld id="{1105B637-3881-4EBD-A1E6-1E923E1EAC5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2198,7 +2212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03474D1A-E819-48AD-A0DB-B989A8D9CC2B}" type="CELLRANGE">
+                    <a:fld id="{79872CBE-4BC6-4867-A022-44B14EBA3DD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2232,7 +2246,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC8E5851-C4CF-4E6B-BA1C-D179235591F0}" type="CELLRANGE">
+                    <a:fld id="{F6A9470E-CBD2-4A6C-A91B-DF6ED4A5D5DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2266,7 +2280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AD1FC92-6FCB-47D9-B55A-C958D64BAC77}" type="CELLRANGE">
+                    <a:fld id="{A5505DBC-4DC7-4D82-B7D4-24B42DE6A024}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2300,7 +2314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD57845B-F325-472E-8AFA-C9269631FD09}" type="CELLRANGE">
+                    <a:fld id="{DFB7003D-52EA-438D-BE79-436C0C099E7A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2334,7 +2348,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA388131-98F5-4387-B43F-4351B4806C81}" type="CELLRANGE">
+                    <a:fld id="{5B9BE296-A5F3-45DF-90B1-C2CF6E7FD2FD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2368,7 +2382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{787D555D-23BE-40CE-9203-9D09E9FE1E46}" type="CELLRANGE">
+                    <a:fld id="{A9FC99A5-F21D-4CBD-8578-607E93EEBBE4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2402,7 +2416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{39EE4C14-1022-4521-B00A-3C48ECE35B1C}" type="CELLRANGE">
+                    <a:fld id="{57951C10-5076-4F3F-BF44-F44E3D8CE8EC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2436,7 +2450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93239FB3-1B8F-4251-8395-B763DC1FCF31}" type="CELLRANGE">
+                    <a:fld id="{3DB8838C-3513-429E-A65A-0E8E6CEF8A3D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2470,7 +2484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE500AF6-4F16-41DF-A5B8-7DE16159281D}" type="CELLRANGE">
+                    <a:fld id="{C4908ED7-AD36-4261-9214-16756F313BC4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2504,7 +2518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE16F8B6-75E2-4EF6-97D2-3AF6095B464F}" type="CELLRANGE">
+                    <a:fld id="{0EED93A5-2ABB-4F87-851C-553B79AED370}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2538,7 +2552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84BDC303-5A0B-4273-996D-D277B0C292A1}" type="CELLRANGE">
+                    <a:fld id="{34832EF6-2150-4AFF-81BF-51903097BBF5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2572,7 +2586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76C27FE7-78E7-480D-B40D-30C2FCA5B065}" type="CELLRANGE">
+                    <a:fld id="{35913A11-BAD8-41C8-8B39-C9CD6AA123E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2606,7 +2620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89B6373F-F9BC-4D88-8EF9-3E3E91A57D0A}" type="CELLRANGE">
+                    <a:fld id="{22881FF6-FCBA-42A9-82E4-9A66622E3934}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2640,7 +2654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCABF0B1-7E02-42DF-B590-5A06CAB6C6D6}" type="CELLRANGE">
+                    <a:fld id="{E2F37EF1-7568-4036-A5FB-58CB74DB4116}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2674,7 +2688,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAF18C23-B7DE-4507-B234-0899F212424C}" type="CELLRANGE">
+                    <a:fld id="{911C9452-D8BD-4A95-9140-66A3E83C34CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4437,10 +4451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3934960F-9A65-4C58-B757-BC73979C20A9}">
-  <dimension ref="A30:G115"/>
+  <dimension ref="A30:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5124,7 +5138,7 @@
         <v>Event 34</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2004</v>
       </c>
@@ -5143,7 +5157,7 @@
         <v>Event 35</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2005</v>
       </c>
@@ -5162,7 +5176,7 @@
         <v>Event 36</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2006</v>
       </c>
@@ -5181,7 +5195,7 @@
         <v>Event 37</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2007</v>
       </c>
@@ -5200,7 +5214,7 @@
         <v>Event 38</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2008</v>
       </c>
@@ -5219,7 +5233,7 @@
         <v>Event 39</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2009</v>
       </c>
@@ -5238,7 +5252,7 @@
         <v>Event 40</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2010</v>
       </c>
@@ -5257,7 +5271,7 @@
         <v>Event 41</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2011</v>
       </c>
@@ -5276,7 +5290,7 @@
         <v>Event 42</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2012</v>
       </c>
@@ -5295,7 +5309,7 @@
         <v>Event 43</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2013</v>
       </c>
@@ -5314,7 +5328,7 @@
         <v>Event 44</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2014</v>
       </c>
@@ -5333,7 +5347,7 @@
         <v>Event 45</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2015</v>
       </c>
@@ -5352,7 +5366,7 @@
         <v>2015 First GMO Meat  Salmon</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2016</v>
       </c>
@@ -5371,7 +5385,7 @@
         <v>Event 47</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2017</v>
       </c>
@@ -5390,7 +5404,7 @@
         <v>Event 48</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2018</v>
       </c>
@@ -5408,8 +5422,11 @@
         <f t="shared" ca="1" si="1"/>
         <v>Event 49</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I79" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2019</v>
       </c>
@@ -5426,6 +5443,9 @@
       <c r="G80" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Event 50</v>
+      </c>
+      <c r="I80" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6034,7 +6054,7 @@
   <dimension ref="B1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
before end of class
</commit_message>
<xml_diff>
--- a/Timeline_ template.xlsx
+++ b/Timeline_ template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annru\Documents\capstone_annrumsey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59F8151-50F4-437A-A16F-0E0899A91EA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A7D06B-53F6-4CC0-9B55-CD8931A19D10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{3E5591EE-1479-4915-B308-C3BDB3157271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3E5591EE-1479-4915-B308-C3BDB3157271}"/>
   </bookViews>
   <sheets>
     <sheet name="Timeline" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
   <si>
     <t>Year</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Mo</t>
   </si>
   <si>
-    <t>Event 1</t>
-  </si>
-  <si>
     <t>Event 2</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Event 10</t>
   </si>
   <si>
-    <t>Event 11</t>
-  </si>
-  <si>
     <t>Event 12</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>Event 20</t>
   </si>
   <si>
-    <t>Event 21</t>
-  </si>
-  <si>
     <t>Event 22</t>
   </si>
   <si>
@@ -139,9 +130,6 @@
     <t>Event 30</t>
   </si>
   <si>
-    <t>Event 31</t>
-  </si>
-  <si>
     <t>Event 32</t>
   </si>
   <si>
@@ -169,9 +157,6 @@
     <t>Event 40</t>
   </si>
   <si>
-    <t>Event 41</t>
-  </si>
-  <si>
     <t>Event 42</t>
   </si>
   <si>
@@ -193,69 +178,27 @@
     <t>Event 49</t>
   </si>
   <si>
-    <t>Event 50</t>
-  </si>
-  <si>
-    <t>Event 51</t>
-  </si>
-  <si>
     <t>Event 54</t>
   </si>
   <si>
-    <t>Event 55</t>
-  </si>
-  <si>
     <t>Event 56</t>
   </si>
   <si>
-    <t>Event 57</t>
-  </si>
-  <si>
-    <t>Event 58</t>
-  </si>
-  <si>
-    <t>Event 59</t>
-  </si>
-  <si>
-    <t>Event 60</t>
-  </si>
-  <si>
-    <t>Event 61</t>
-  </si>
-  <si>
     <t>Event 62</t>
   </si>
   <si>
     <t>Event 63</t>
   </si>
   <si>
-    <t>Event 64</t>
-  </si>
-  <si>
-    <t>Event 65</t>
-  </si>
-  <si>
-    <t>Event 66</t>
-  </si>
-  <si>
     <t>Event 67</t>
   </si>
   <si>
-    <t>Event 68</t>
-  </si>
-  <si>
     <t>Event 69</t>
   </si>
   <si>
     <t>Event 70</t>
   </si>
   <si>
-    <t>Event 71</t>
-  </si>
-  <si>
-    <t>Event 72</t>
-  </si>
-  <si>
     <t>Event 73</t>
   </si>
   <si>
@@ -271,16 +214,7 @@
     <t>Event 77</t>
   </si>
   <si>
-    <t>Event 78</t>
-  </si>
-  <si>
-    <t>Event 79</t>
-  </si>
-  <si>
     <t>Event 80</t>
-  </si>
-  <si>
-    <t>Event 81</t>
   </si>
   <si>
     <t>Event 82</t>
@@ -483,12 +417,39 @@
   <si>
     <t>FDA deactivation of an import alert on genetically engineered salmon</t>
   </si>
+  <si>
+    <t>Projected Populaton 331,002,651</t>
+  </si>
+  <si>
+    <t>Census Populaton 308,745,538</t>
+  </si>
+  <si>
+    <t>Census Populaton 281,401,351</t>
+  </si>
+  <si>
+    <t>Census Populaton 248,709,873</t>
+  </si>
+  <si>
+    <t>Census Populaton 226,545,805</t>
+  </si>
+  <si>
+    <t>Census Populaton 203,211,926</t>
+  </si>
+  <si>
+    <t>Projected Populaton 349,641,876</t>
+  </si>
+  <si>
+    <t>Projected Populaton 366,572,154</t>
+  </si>
+  <si>
+    <t>Projected Populaton 379,419,102</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -562,6 +523,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -584,7 +550,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -611,6 +577,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -645,7 +618,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="1.7695820161573585E-2"/>
+          <c:y val="3.3950617283950615E-2"/>
+          <c:w val="0.96812082894274676"/>
+          <c:h val="0.9320987654320988"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -682,7 +665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEF157FB-4593-4D33-B6ED-6A0F2E9E4DFE}" type="CELLRANGE">
+                    <a:fld id="{A1D79CFC-0669-4DFE-BB2D-516CDBB97E4E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -716,7 +699,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DABE872-DE0D-4CE7-A201-4352A46CBDDB}" type="CELLRANGE">
+                    <a:fld id="{CD76F921-E6D2-4250-B477-3F7937E0589E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -750,7 +733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7215229C-AD75-4093-BC6E-E0629B7D3B41}" type="CELLRANGE">
+                    <a:fld id="{0CF2D628-A0FA-4DFA-9818-707DE5FB485F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -784,7 +767,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C0060A9-1669-4B5E-A638-4B09F38EA961}" type="CELLRANGE">
+                    <a:fld id="{31131255-B828-4966-829D-43E13058975F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -818,7 +801,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B789163-6573-4E20-A19E-B5EB965010DB}" type="CELLRANGE">
+                    <a:fld id="{D5CE357C-90CC-47EA-BFB0-2314B882F225}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -852,7 +835,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19F98B79-E674-4880-9CB6-E193EA7CF634}" type="CELLRANGE">
+                    <a:fld id="{42BE8F11-2492-4C22-A2A6-740B61B53A2A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -886,7 +869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6029CA03-AEEC-43B6-B0E0-6C6A0BCDCED3}" type="CELLRANGE">
+                    <a:fld id="{D8D9AAF3-C7EA-4338-889C-E438DE6D7340}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -920,7 +903,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FD3CE55-F9E6-4939-AF3C-E183EF52083E}" type="CELLRANGE">
+                    <a:fld id="{BB1D9E25-F548-4011-BDFE-5D4D863B9D4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -954,7 +937,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28A9ECA4-E759-48CC-B190-C2A64BA775C0}" type="CELLRANGE">
+                    <a:fld id="{02CA3E5F-680F-49E2-9B72-6118C7A113F8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -988,7 +971,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDAF7600-CD0D-47EA-A5F1-D9A134687532}" type="CELLRANGE">
+                    <a:fld id="{F740033C-2EC3-4F92-A2DE-556915799DD9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1022,7 +1005,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AAE52DF-D2BA-4840-A76E-1CAAF55B6AE2}" type="CELLRANGE">
+                    <a:fld id="{17980427-A89E-4BE5-A0B4-D4EF1444DAFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1056,7 +1039,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E35C1F1-85E1-4C7C-9A23-DFB13D4B6FC7}" type="CELLRANGE">
+                    <a:fld id="{1344C3FD-56C0-43D5-93C5-8086A65FFF1D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1090,7 +1073,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8F641A8-6F5F-4F89-9C9B-B00C99D4CB97}" type="CELLRANGE">
+                    <a:fld id="{2892ECD1-787B-4444-945C-1899457696D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1124,7 +1107,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB0A50A7-FCEA-4EAA-9BEA-DDDB135D23EB}" type="CELLRANGE">
+                    <a:fld id="{AE576867-0CA2-4DFE-9EA5-8F11D8FC1CC6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1158,7 +1141,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5F2F0FB-3A2A-42CA-B748-5DE339F55766}" type="CELLRANGE">
+                    <a:fld id="{E357F714-BE2F-45AC-98FD-BECC071E7697}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1192,7 +1175,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5DA63A12-F687-4923-83AA-8054AB1DE90F}" type="CELLRANGE">
+                    <a:fld id="{DC041094-250E-4B14-9D9B-5606A67D5E6A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1226,7 +1209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C24CD87-B3F2-48DC-B22C-F89A7962D5E4}" type="CELLRANGE">
+                    <a:fld id="{670A4DFB-C865-40FB-BC58-7A43D1FD8B8A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1260,7 +1243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C05EBD74-692F-4D62-A822-04CAB04AF405}" type="CELLRANGE">
+                    <a:fld id="{D538846C-9F37-4393-A4FF-2E1B9076EA1B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1294,7 +1277,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{224F08B4-9B88-4EC4-9764-C4863A58A99D}" type="CELLRANGE">
+                    <a:fld id="{CE3CA1D7-DFEC-4B3F-AD50-F5BB71459ADF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1328,7 +1311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC8FBE75-4FA5-4380-A127-E3DAC4A09882}" type="CELLRANGE">
+                    <a:fld id="{F5A67C7B-6847-4C85-B9A2-9A3E2ACDB8DB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1362,7 +1345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{570AC00F-4915-4A29-A5D7-C17C7A37B1D7}" type="CELLRANGE">
+                    <a:fld id="{F2ED4214-4931-45FC-AC95-D9893F86EC47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1396,7 +1379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E507077B-1345-48D1-B6DD-7EAEA7EFE85D}" type="CELLRANGE">
+                    <a:fld id="{BB4E271D-0502-48AA-8252-3774E28B9C0A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1430,7 +1413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E5EF788-1097-4809-8A7F-F9EBF6B329CD}" type="CELLRANGE">
+                    <a:fld id="{8B1509BF-5E13-4399-B97B-1D499C34EC72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1464,7 +1447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD01CBB6-D322-417B-A5DB-F66C00FE01D1}" type="CELLRANGE">
+                    <a:fld id="{8A51FAF1-EE03-4E62-BB90-1C722CE08397}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1498,7 +1481,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{554BFF2B-B9FB-467C-8C07-C8F56C147F18}" type="CELLRANGE">
+                    <a:fld id="{32858929-74C6-45E4-A83C-DF89C12A922B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1532,7 +1515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA89D949-05D9-4B34-88C4-A79A6E309949}" type="CELLRANGE">
+                    <a:fld id="{DCB795AC-04F8-47E6-87B4-AD56E33A8B32}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1566,7 +1549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{702843F7-A211-41FF-ACD3-7930FBC6202A}" type="CELLRANGE">
+                    <a:fld id="{9665B5D7-FC16-4B9A-BAFC-C8DCE16F3883}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1600,7 +1583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72EEDD67-5853-4368-879E-2051AA3A4C4D}" type="CELLRANGE">
+                    <a:fld id="{095D6273-334F-4E6F-91F1-F93015757A33}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1634,7 +1617,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB26A554-78EB-412B-B5CB-E518F396DA57}" type="CELLRANGE">
+                    <a:fld id="{DB7A2EF4-9093-48FC-8F3B-8324232F9468}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1668,7 +1651,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{457441B7-BEAF-497A-B5DD-C93C62E7E8C0}" type="CELLRANGE">
+                    <a:fld id="{7D753F2E-29D2-4556-AFAB-A6A6507D7B39}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1702,7 +1685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3258D22F-9576-47E7-ADDC-77F590CE5422}" type="CELLRANGE">
+                    <a:fld id="{7AAEEE67-C6FA-4D2E-B3E7-A3307964E534}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1736,7 +1719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2399F71D-169F-4636-BBF9-8F1FE08937FF}" type="CELLRANGE">
+                    <a:fld id="{C16D6DC4-2443-4AD9-83DB-F4A1D917F896}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1770,7 +1753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{423ECD27-115D-4CD7-BA5A-0C11682D5EA8}" type="CELLRANGE">
+                    <a:fld id="{B51A53A3-44E0-437D-9D0E-D3D674A61822}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1804,7 +1787,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B3B5C18-DC4F-4760-853D-FACE073F07AB}" type="CELLRANGE">
+                    <a:fld id="{9D5A124A-8914-43FB-8229-A82B38348B52}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1838,7 +1821,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5304F656-8DC1-47D5-8D9B-C9343E5D21FD}" type="CELLRANGE">
+                    <a:fld id="{9E2CA3A4-5CF5-4D61-B33E-3386F63E29EF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1872,7 +1855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{874971DA-A155-4D3F-9EEE-EEA0DA7E9291}" type="CELLRANGE">
+                    <a:fld id="{AE001725-27F1-489D-AC24-D427BCD6B031}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1906,7 +1889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13EDF590-DE9B-4C64-8109-3F5700EBFF5E}" type="CELLRANGE">
+                    <a:fld id="{460486E2-C104-4B00-89C6-CC4427ACF439}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1940,7 +1923,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C126BC2-0983-4DDF-A560-1F3A89AD07EE}" type="CELLRANGE">
+                    <a:fld id="{38C3396B-78CC-43F7-8B53-98E6AFD34F4A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1974,7 +1957,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6FE13CB-6347-44EC-A0F0-34F49303F5C6}" type="CELLRANGE">
+                    <a:fld id="{67FDEA87-F05C-45FB-A7B9-C117BDBA18DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2008,7 +1991,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B72B7B4-EED1-4293-ABE5-751562B422F8}" type="CELLRANGE">
+                    <a:fld id="{217258DE-37EF-45E9-AD07-5E751CA122DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2042,7 +2025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB4130CB-1439-4A78-9821-3277D6FA6657}" type="CELLRANGE">
+                    <a:fld id="{70C36138-6EEE-4845-86C1-3F53A765F9C8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2076,7 +2059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B70977E5-E04F-4E93-8174-238705DE5A1A}" type="CELLRANGE">
+                    <a:fld id="{23313194-F89C-4C28-A670-2F65B9F6C08F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2110,7 +2093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{354B5F78-A02C-4555-B489-8BE5C7E4BB9E}" type="CELLRANGE">
+                    <a:fld id="{66B8A288-E5A9-4BD9-AD54-4A182DD9A89E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2144,7 +2127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C62AAC3-E6E5-4DF8-A0DD-1891DC68AB85}" type="CELLRANGE">
+                    <a:fld id="{55C15F8E-B686-4670-84A9-C16888462780}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2178,7 +2161,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1105B637-3881-4EBD-A1E6-1E923E1EAC5A}" type="CELLRANGE">
+                    <a:fld id="{67121C33-48C0-416C-A1B4-4B2AEC9E3DB1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2212,7 +2195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79872CBE-4BC6-4867-A022-44B14EBA3DD5}" type="CELLRANGE">
+                    <a:fld id="{2730DD7B-F2A6-42AB-A247-9E698E59439F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2246,7 +2229,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F6A9470E-CBD2-4A6C-A91B-DF6ED4A5D5DE}" type="CELLRANGE">
+                    <a:fld id="{2FCE6931-B219-4BFB-9399-F9E7AE9216B5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2280,7 +2263,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A5505DBC-4DC7-4D82-B7D4-24B42DE6A024}" type="CELLRANGE">
+                    <a:fld id="{4E721266-8427-42EC-9867-49DB8D06235C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2314,7 +2297,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFB7003D-52EA-438D-BE79-436C0C099E7A}" type="CELLRANGE">
+                    <a:fld id="{9429563C-0556-4D83-BF19-72BC8E6CB923}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2348,7 +2331,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B9BE296-A5F3-45DF-90B1-C2CF6E7FD2FD}" type="CELLRANGE">
+                    <a:fld id="{129E86EA-7E84-4E51-B00E-CD77A7D6E3B2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2382,7 +2365,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9FC99A5-F21D-4CBD-8578-607E93EEBBE4}" type="CELLRANGE">
+                    <a:fld id="{AE854FCA-7568-4751-8589-0ED8FFB32446}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2416,7 +2399,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57951C10-5076-4F3F-BF44-F44E3D8CE8EC}" type="CELLRANGE">
+                    <a:fld id="{863363AB-F191-4CEA-987F-D6E82089E96F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2450,7 +2433,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DB8838C-3513-429E-A65A-0E8E6CEF8A3D}" type="CELLRANGE">
+                    <a:fld id="{5FF9B458-CD5F-4B73-8227-779316B17064}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2484,7 +2467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4908ED7-AD36-4261-9214-16756F313BC4}" type="CELLRANGE">
+                    <a:fld id="{F5C3EDFB-FD00-4799-92D6-8CD77EC943AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2518,7 +2501,35 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EED93A5-2ABB-4F87-851C-553B79AED370}" type="CELLRANGE">
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000037-32D4-4891-B46F-D74D6930CA79}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="55"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3AA27308-D31D-427F-8C65-8527E2905210}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2541,18 +2552,130 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000037-32D4-4891-B46F-D74D6930CA79}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="55"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{34832EF6-2150-4AFF-81BF-51903097BBF5}" type="CELLRANGE">
+                  <c16:uniqueId val="{00000038-32D4-4891-B46F-D74D6930CA79}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="56"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000039-32D4-4891-B46F-D74D6930CA79}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="57"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000003A-32D4-4891-B46F-D74D6930CA79}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="58"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000003B-32D4-4891-B46F-D74D6930CA79}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="59"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000003C-32D4-4891-B46F-D74D6930CA79}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="60"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{15ED807C-5F9C-49D3-A749-CF43F396F9F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2575,18 +2698,18 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000038-32D4-4891-B46F-D74D6930CA79}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="56"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{35913A11-BAD8-41C8-8B39-C9CD6AA123E1}" type="CELLRANGE">
+                  <c16:uniqueId val="{00000000-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="61"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{65E2B009-20D8-4FF7-A2D5-080A3A1F9AD4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2609,18 +2732,18 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000039-32D4-4891-B46F-D74D6930CA79}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="57"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{22881FF6-FCBA-42A9-82E4-9A66622E3934}" type="CELLRANGE">
+                  <c16:uniqueId val="{00000001-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="62"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3B609C81-44DC-4105-9E33-614EA3249B6B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2643,18 +2766,102 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000003A-32D4-4891-B46F-D74D6930CA79}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="58"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{E2F37EF1-7568-4036-A5FB-58CB74DB4116}" type="CELLRANGE">
+                  <c16:uniqueId val="{00000002-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="63"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="64"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="65"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="66"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{BD2290E0-0C6F-4E3A-BCF8-AF6451B413F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2677,18 +2884,46 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000003B-32D4-4891-B46F-D74D6930CA79}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="59"/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:fld id="{911C9452-D8BD-4A95-9140-66A3E83C34CE}" type="CELLRANGE">
+                  <c16:uniqueId val="{00000006-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="67"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="68"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FA5398A9-009B-4E25-AC5F-6AB0D3E832C1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2711,7 +2946,465 @@
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000003C-32D4-4891-B46F-D74D6930CA79}"/>
+                  <c16:uniqueId val="{00000008-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="69"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C402ECC9-60CE-417F-9429-87946E6C7625}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="70"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4C5DC74E-F565-4D69-A098-082855385829}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="71"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="72"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2D11F772-762E-41B9-85CC-E3F6BED1C955}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="73"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{53F7FA00-E88C-4FC7-A785-AEAC35B105A0}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="74"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{068CF5CC-7277-4007-B2A2-32FC544714BD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="75"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3F702B9E-FB5C-4C38-A258-31FFEAE92628}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="76"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{88B5C58E-37FE-4F1E-941F-AF3A7E4EBDC0}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="77"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="78"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="79"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{90C4F0E3-FB45-450C-B0D7-847542C85CBD}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="80"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C664A6EA-C256-4884-813F-55C3203788CE}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="81"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{22246D76-EC58-4764-8C74-4FD7B1395B3D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="82"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CB9E284B-EA70-44B0-A22D-4C72CE6BC559}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-99EE-4054-BA8E-ACEC5A3E2DF6}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -2822,10 +3515,10 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Timeline!$F$31:$F$90</c:f>
+              <c:f>Timeline!$F$31:$F$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="83"/>
                 <c:pt idx="0">
                   <c:v>1970</c:v>
                 </c:pt>
@@ -3005,16 +3698,85 @@
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Timeline!$E$31:$E$90</c:f>
+              <c:f>Timeline!$E$31:$E$113</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
+                <c:ptCount val="83"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -3151,7 +3913,7 @@
                   <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>50</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>-75</c:v>
@@ -3177,23 +3939,56 @@
                 <c:pt idx="53">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="54">
-                  <c:v>75</c:v>
-                </c:pt>
                 <c:pt idx="55">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="56">
-                  <c:v>-100</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>-90</c:v>
-                </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="60">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="61">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-75</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3202,11 +3997,11 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>Timeline!$G$31:$G$90</c15:f>
+                <c15:f>Timeline!$G$31:$G$113</c15:f>
                 <c15:dlblRangeCache>
-                  <c:ptCount val="60"/>
+                  <c:ptCount val="83"/>
                   <c:pt idx="0">
-                    <c:v>Event 1</c:v>
+                    <c:v>Census Populaton 203,211,926</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>Event 2</c:v>
@@ -3236,7 +4031,7 @@
                     <c:v>Event 10</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>Event 11</c:v>
+                    <c:v>Census Populaton 226,545,805</c:v>
                   </c:pt>
                   <c:pt idx="11">
                     <c:v>Event 12</c:v>
@@ -3266,7 +4061,7 @@
                     <c:v>Event 20</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>Event 21</c:v>
+                    <c:v>Census Populaton 248,709,873</c:v>
                   </c:pt>
                   <c:pt idx="21">
                     <c:v>Event 22</c:v>
@@ -3296,7 +4091,7 @@
                     <c:v>Event 30</c:v>
                   </c:pt>
                   <c:pt idx="30">
-                    <c:v>Event 31</c:v>
+                    <c:v>Census Populaton 281,401,351</c:v>
                   </c:pt>
                   <c:pt idx="31">
                     <c:v>Event 32</c:v>
@@ -3326,7 +4121,7 @@
                     <c:v>Event 40</c:v>
                   </c:pt>
                   <c:pt idx="40">
-                    <c:v>Event 41</c:v>
+                    <c:v>Census Populaton 308,745,538</c:v>
                   </c:pt>
                   <c:pt idx="41">
                     <c:v>Event 42</c:v>
@@ -3353,10 +4148,10 @@
                     <c:v>Event 49</c:v>
                   </c:pt>
                   <c:pt idx="49">
-                    <c:v>Event 50</c:v>
+                    <c:v>FDA deactivation of an import alert on genetically engineered salmon</c:v>
                   </c:pt>
                   <c:pt idx="50">
-                    <c:v>Event 51</c:v>
+                    <c:v>Projected Populaton 331,002,651</c:v>
                   </c:pt>
                   <c:pt idx="51">
                     <c:v>CRISPR potential for COVID-19</c:v>
@@ -3367,23 +4162,56 @@
                   <c:pt idx="53">
                     <c:v>Event 54</c:v>
                   </c:pt>
-                  <c:pt idx="54">
-                    <c:v>Event 55</c:v>
-                  </c:pt>
                   <c:pt idx="55">
                     <c:v>Event 56</c:v>
                   </c:pt>
-                  <c:pt idx="56">
-                    <c:v>Event 57</c:v>
+                  <c:pt idx="60">
+                    <c:v>Projected Populaton 349,641,876</c:v>
                   </c:pt>
-                  <c:pt idx="57">
-                    <c:v>Event 58</c:v>
+                  <c:pt idx="61">
+                    <c:v>Event 62</c:v>
                   </c:pt>
-                  <c:pt idx="58">
-                    <c:v>Event 59</c:v>
+                  <c:pt idx="62">
+                    <c:v>Event 63</c:v>
                   </c:pt>
-                  <c:pt idx="59">
-                    <c:v>Event 60</c:v>
+                  <c:pt idx="66">
+                    <c:v>Event 67</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>Event 69</c:v>
+                  </c:pt>
+                  <c:pt idx="69">
+                    <c:v>Event 70</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>Projected Populaton 366,572,154</c:v>
+                  </c:pt>
+                  <c:pt idx="72">
+                    <c:v>Event 73</c:v>
+                  </c:pt>
+                  <c:pt idx="73">
+                    <c:v>Event 74</c:v>
+                  </c:pt>
+                  <c:pt idx="74">
+                    <c:v>Event 75</c:v>
+                  </c:pt>
+                  <c:pt idx="75">
+                    <c:v>Event 76</c:v>
+                  </c:pt>
+                  <c:pt idx="76">
+                    <c:v>Event 77</c:v>
+                  </c:pt>
+                  <c:pt idx="79">
+                    <c:v>Event 80</c:v>
+                  </c:pt>
+                  <c:pt idx="80">
+                    <c:v>Projected Populaton 379,419,102</c:v>
+                  </c:pt>
+                  <c:pt idx="81">
+                    <c:v>Event 82</c:v>
+                  </c:pt>
+                  <c:pt idx="82">
+                    <c:v>Event 83</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -4453,13 +5281,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3934960F-9A65-4C58-B757-BC73979C20A9}">
   <dimension ref="A30:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L82" sqref="L82"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="12" customWidth="1"/>
     <col min="7" max="7" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4479,7 +5308,7 @@
       <c r="E30" t="s">
         <v>3</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="12" t="s">
         <v>4</v>
       </c>
       <c r="G30" t="s">
@@ -4491,12 +5320,12 @@
         <v>1970</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="E31">
         <v>50</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="13">
         <f ca="1">OFFSET($A$30,ROW()-ROW($A$30),0,1,1)
  + ( DATE(1900,IF(OFFSET($B$30,ROW()-ROW($B$30),0,1,1)="", 1,
 OFFSET($B$30,ROW()-ROW($B$30),0,1,1)),0)
@@ -4505,7 +5334,7 @@
       </c>
       <c r="G31" s="1" t="str">
         <f ca="1">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
-        <v>Event 1</v>
+        <v>Census Populaton 203,211,926</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -4513,12 +5342,12 @@
         <v>1971</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32">
         <v>-75</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="13">
         <f t="shared" ref="F32:F95" ca="1" si="0">OFFSET($A$30,ROW()-ROW($A$30),0,1,1)
  + ( DATE(1900,IF(OFFSET($B$30,ROW()-ROW($B$30),0,1,1)="", 1,
 OFFSET($B$30,ROW()-ROW($B$30),0,1,1)),0)
@@ -4535,12 +5364,12 @@
         <v>1972</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33">
         <v>-40</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1972</v>
       </c>
@@ -4554,12 +5383,12 @@
         <v>1973</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E34">
         <v>100</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1973</v>
       </c>
@@ -4573,12 +5402,12 @@
         <v>1974</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35">
         <v>75</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1974</v>
       </c>
@@ -4592,12 +5421,12 @@
         <v>1975</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E36">
         <v>50</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F36" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1975</v>
       </c>
@@ -4611,12 +5440,12 @@
         <v>1976</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E37">
         <v>-75</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1976</v>
       </c>
@@ -4630,12 +5459,12 @@
         <v>1977</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E38">
         <v>-40</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1977</v>
       </c>
@@ -4649,12 +5478,12 @@
         <v>1978</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39">
         <v>100</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1978</v>
       </c>
@@ -4668,12 +5497,12 @@
         <v>1979</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E40">
         <v>-100</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1979</v>
       </c>
@@ -4687,18 +5516,18 @@
         <v>1980</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
       <c r="E41">
         <v>50</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1980</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 11</v>
+        <v>Census Populaton 226,545,805</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -4706,12 +5535,12 @@
         <v>1981</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E42">
         <v>-75</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1981</v>
       </c>
@@ -4725,12 +5554,12 @@
         <v>1982</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="E43">
         <v>-40</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1982</v>
       </c>
@@ -4744,12 +5573,12 @@
         <v>1983</v>
       </c>
       <c r="D44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E44">
         <v>100</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1983</v>
       </c>
@@ -4763,12 +5592,12 @@
         <v>1984</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E45">
         <v>75</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F45" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1984</v>
       </c>
@@ -4782,12 +5611,12 @@
         <v>1985</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E46">
         <v>50</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F46" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1985</v>
       </c>
@@ -4801,12 +5630,12 @@
         <v>1986</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E47">
         <v>-100</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1986</v>
       </c>
@@ -4820,12 +5649,12 @@
         <v>1987</v>
       </c>
       <c r="D48" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="E48">
         <v>-75</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F48" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1987</v>
       </c>
@@ -4839,12 +5668,12 @@
         <v>1988</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E49">
         <v>100</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F49" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1988</v>
       </c>
@@ -4858,12 +5687,12 @@
         <v>1989</v>
       </c>
       <c r="D50" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E50">
         <v>-100</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F50" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1989</v>
       </c>
@@ -4877,18 +5706,18 @@
         <v>1990</v>
       </c>
       <c r="D51" t="s">
-        <v>25</v>
+        <v>97</v>
       </c>
       <c r="E51">
         <v>50</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F51" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1990</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 21</v>
+        <v>Census Populaton 248,709,873</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -4896,12 +5725,12 @@
         <v>1991</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E52">
         <v>-40</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F52" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1991</v>
       </c>
@@ -4915,12 +5744,12 @@
         <v>1992</v>
       </c>
       <c r="D53" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E53">
         <v>-40</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F53" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1992</v>
       </c>
@@ -4934,12 +5763,12 @@
         <v>1993</v>
       </c>
       <c r="D54" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E54">
         <v>100</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F54" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1993</v>
       </c>
@@ -4953,12 +5782,12 @@
         <v>1994</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E55">
         <v>75</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F55" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1994</v>
       </c>
@@ -4972,12 +5801,12 @@
         <v>1995</v>
       </c>
       <c r="D56" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E56">
         <v>50</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F56" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1995</v>
       </c>
@@ -4991,12 +5820,12 @@
         <v>1996</v>
       </c>
       <c r="D57" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E57">
         <v>-75</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1996</v>
       </c>
@@ -5010,12 +5839,12 @@
         <v>1997</v>
       </c>
       <c r="D58" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E58">
         <v>-40</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F58" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1997</v>
       </c>
@@ -5029,12 +5858,12 @@
         <v>1998</v>
       </c>
       <c r="D59" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E59">
         <v>100</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F59" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1998</v>
       </c>
@@ -5048,12 +5877,12 @@
         <v>1999</v>
       </c>
       <c r="D60" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E60">
         <v>-100</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>1999</v>
       </c>
@@ -5067,18 +5896,18 @@
         <v>2000</v>
       </c>
       <c r="D61" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="E61">
         <v>50</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F61" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2000</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 31</v>
+        <v>Census Populaton 281,401,351</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -5086,12 +5915,12 @@
         <v>2001</v>
       </c>
       <c r="D62" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E62">
         <v>-75</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F62" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2001</v>
       </c>
@@ -5105,12 +5934,12 @@
         <v>2002</v>
       </c>
       <c r="D63" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E63">
         <v>-40</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F63" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2002</v>
       </c>
@@ -5124,12 +5953,12 @@
         <v>2003</v>
       </c>
       <c r="D64" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E64">
         <v>100</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F64" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2003</v>
       </c>
@@ -5143,12 +5972,12 @@
         <v>2004</v>
       </c>
       <c r="D65" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E65">
         <v>75</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2004</v>
       </c>
@@ -5162,12 +5991,12 @@
         <v>2005</v>
       </c>
       <c r="D66" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E66">
         <v>50</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2005</v>
       </c>
@@ -5181,12 +6010,12 @@
         <v>2006</v>
       </c>
       <c r="D67" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E67">
         <v>-75</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2006</v>
       </c>
@@ -5200,12 +6029,12 @@
         <v>2007</v>
       </c>
       <c r="D68" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E68">
         <v>-40</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2007</v>
       </c>
@@ -5219,12 +6048,12 @@
         <v>2008</v>
       </c>
       <c r="D69" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E69">
         <v>100</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F69" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2008</v>
       </c>
@@ -5238,12 +6067,12 @@
         <v>2009</v>
       </c>
       <c r="D70" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E70">
         <v>-100</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F70" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2009</v>
       </c>
@@ -5257,18 +6086,18 @@
         <v>2010</v>
       </c>
       <c r="D71" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="E71">
         <v>50</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2010</v>
       </c>
       <c r="G71" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 41</v>
+        <v>Census Populaton 308,745,538</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -5276,12 +6105,12 @@
         <v>2011</v>
       </c>
       <c r="D72" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E72">
         <v>-75</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2011</v>
       </c>
@@ -5295,12 +6124,12 @@
         <v>2012</v>
       </c>
       <c r="D73" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E73">
         <v>-40</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2012</v>
       </c>
@@ -5314,12 +6143,12 @@
         <v>2013</v>
       </c>
       <c r="D74" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E74">
         <v>100</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2013</v>
       </c>
@@ -5333,12 +6162,12 @@
         <v>2014</v>
       </c>
       <c r="D75" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E75">
         <v>75</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F75" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2014</v>
       </c>
@@ -5352,12 +6181,12 @@
         <v>2015</v>
       </c>
       <c r="D76" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E76">
-        <v>50</v>
-      </c>
-      <c r="F76" s="1">
+        <v>100</v>
+      </c>
+      <c r="F76" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2015</v>
       </c>
@@ -5371,12 +6200,12 @@
         <v>2016</v>
       </c>
       <c r="D77" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E77">
         <v>-75</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F77" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2016</v>
       </c>
@@ -5390,12 +6219,12 @@
         <v>2017</v>
       </c>
       <c r="D78" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E78">
         <v>-40</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F78" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2017</v>
       </c>
@@ -5409,12 +6238,12 @@
         <v>2018</v>
       </c>
       <c r="D79" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E79">
         <v>100</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F79" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2018</v>
       </c>
@@ -5423,29 +6252,30 @@
         <v>Event 49</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2019</v>
       </c>
-      <c r="D80" t="s">
-        <v>52</v>
+      <c r="D80" t="str">
+        <f>I80</f>
+        <v>FDA deactivation of an import alert on genetically engineered salmon</v>
       </c>
       <c r="E80">
         <v>-100</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F80" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2019</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 50</v>
+        <v>FDA deactivation of an import alert on genetically engineered salmon</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -5453,18 +6283,18 @@
         <v>2020</v>
       </c>
       <c r="D81" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="E81">
         <v>75</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F81" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2020</v>
       </c>
       <c r="G81" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 51</v>
+        <v>Projected Populaton 331,002,651</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -5472,12 +6302,12 @@
         <v>2021</v>
       </c>
       <c r="D82" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="E82">
         <v>-75</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F82" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2021</v>
       </c>
@@ -5491,12 +6321,12 @@
         <v>2022</v>
       </c>
       <c r="D83" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="E83">
         <v>-40</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F83" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2022</v>
       </c>
@@ -5510,12 +6340,12 @@
         <v>2023</v>
       </c>
       <c r="D84" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E84">
         <v>100</v>
       </c>
-      <c r="F84" s="1">
+      <c r="F84" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2023</v>
       </c>
@@ -5528,32 +6358,23 @@
       <c r="A85">
         <v>2024</v>
       </c>
-      <c r="D85" t="s">
-        <v>55</v>
-      </c>
-      <c r="E85">
-        <v>75</v>
-      </c>
-      <c r="F85" s="1">
+      <c r="F85" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2024</v>
       </c>
-      <c r="G85" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 55</v>
-      </c>
+      <c r="G85" s="1"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2025</v>
       </c>
       <c r="D86" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="E86">
         <v>50</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F86" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2025</v>
       </c>
@@ -5566,92 +6387,59 @@
       <c r="A87">
         <v>2026</v>
       </c>
-      <c r="D87" t="s">
-        <v>57</v>
-      </c>
-      <c r="E87">
-        <v>-100</v>
-      </c>
-      <c r="F87" s="1">
+      <c r="F87" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2026</v>
       </c>
-      <c r="G87" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 57</v>
-      </c>
+      <c r="G87" s="1"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2027</v>
       </c>
-      <c r="D88" t="s">
-        <v>58</v>
-      </c>
-      <c r="E88">
-        <v>-90</v>
-      </c>
-      <c r="F88" s="1">
+      <c r="F88" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2027</v>
       </c>
-      <c r="G88" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 58</v>
-      </c>
+      <c r="G88" s="1"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2028</v>
       </c>
-      <c r="D89" t="s">
-        <v>59</v>
-      </c>
-      <c r="E89">
-        <v>100</v>
-      </c>
-      <c r="F89" s="1">
+      <c r="F89" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2028</v>
       </c>
-      <c r="G89" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 59</v>
-      </c>
+      <c r="G89" s="14"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2029</v>
       </c>
-      <c r="D90" t="s">
-        <v>60</v>
-      </c>
-      <c r="E90">
-        <v>-40</v>
-      </c>
-      <c r="F90" s="1">
+      <c r="F90" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2029</v>
       </c>
-      <c r="G90" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 60</v>
-      </c>
+      <c r="G90" s="1"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2030</v>
       </c>
       <c r="D91" t="s">
-        <v>61</v>
-      </c>
-      <c r="F91" s="1">
+        <v>100</v>
+      </c>
+      <c r="E91">
+        <v>100</v>
+      </c>
+      <c r="F91" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2030</v>
       </c>
       <c r="G91" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Event 61</v>
+        <v>Projected Populaton 349,641,876</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -5659,9 +6447,12 @@
         <v>2031</v>
       </c>
       <c r="D92" t="s">
-        <v>62</v>
-      </c>
-      <c r="F92" s="1">
+        <v>49</v>
+      </c>
+      <c r="E92">
+        <v>75</v>
+      </c>
+      <c r="F92" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2031</v>
       </c>
@@ -5675,9 +6466,12 @@
         <v>2032</v>
       </c>
       <c r="D93" t="s">
-        <v>63</v>
-      </c>
-      <c r="F93" s="1">
+        <v>50</v>
+      </c>
+      <c r="E93">
+        <v>50</v>
+      </c>
+      <c r="F93" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2032</v>
       </c>
@@ -5690,66 +6484,51 @@
       <c r="A94">
         <v>2033</v>
       </c>
-      <c r="D94" t="s">
-        <v>64</v>
-      </c>
-      <c r="F94" s="1">
+      <c r="F94" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2033</v>
       </c>
-      <c r="G94" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 64</v>
-      </c>
+      <c r="G94" s="1"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2034</v>
       </c>
-      <c r="D95" t="s">
-        <v>65</v>
-      </c>
-      <c r="F95" s="1">
+      <c r="F95" s="13">
         <f t="shared" ca="1" si="0"/>
         <v>2034</v>
       </c>
-      <c r="G95" s="1" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Event 65</v>
-      </c>
+      <c r="G95" s="1"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2035</v>
       </c>
-      <c r="D96" t="s">
-        <v>66</v>
-      </c>
-      <c r="F96" s="1">
+      <c r="F96" s="13">
         <f t="shared" ref="F96:F115" ca="1" si="2">OFFSET($A$30,ROW()-ROW($A$30),0,1,1)
  + ( DATE(1900,IF(OFFSET($B$30,ROW()-ROW($B$30),0,1,1)="", 1,
 OFFSET($B$30,ROW()-ROW($B$30),0,1,1)),0)
  + OFFSET($C$30,ROW()-ROW($C$30),0,1,1) ) / 365.25</f>
         <v>2035</v>
       </c>
-      <c r="G96" s="1" t="str">
-        <f t="shared" ref="G96:G115" ca="1" si="3">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
-        <v>Event 66</v>
-      </c>
+      <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2036</v>
       </c>
       <c r="D97" t="s">
-        <v>67</v>
-      </c>
-      <c r="F97" s="1">
+        <v>51</v>
+      </c>
+      <c r="E97">
+        <v>-40</v>
+      </c>
+      <c r="F97" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2036</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ref="G96:G115" ca="1" si="3">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
         <v>Event 67</v>
       </c>
     </row>
@@ -5757,26 +6536,23 @@
       <c r="A98">
         <v>2037</v>
       </c>
-      <c r="D98" t="s">
-        <v>68</v>
-      </c>
-      <c r="F98" s="1">
+      <c r="F98" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2037</v>
       </c>
-      <c r="G98" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>Event 68</v>
-      </c>
+      <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2038</v>
       </c>
       <c r="D99" t="s">
-        <v>69</v>
-      </c>
-      <c r="F99" s="1">
+        <v>52</v>
+      </c>
+      <c r="E99">
+        <v>75</v>
+      </c>
+      <c r="F99" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2038</v>
       </c>
@@ -5790,9 +6566,12 @@
         <v>2039</v>
       </c>
       <c r="D100" t="s">
-        <v>70</v>
-      </c>
-      <c r="F100" s="1">
+        <v>53</v>
+      </c>
+      <c r="E100">
+        <v>50</v>
+      </c>
+      <c r="F100" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2039</v>
       </c>
@@ -5806,41 +6585,41 @@
         <v>2040</v>
       </c>
       <c r="D101" t="s">
-        <v>71</v>
-      </c>
-      <c r="F101" s="1">
+        <v>101</v>
+      </c>
+      <c r="E101">
+        <v>-75</v>
+      </c>
+      <c r="F101" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2040</v>
       </c>
       <c r="G101" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Event 71</v>
+        <v>Projected Populaton 366,572,154</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2041</v>
       </c>
-      <c r="D102" t="s">
-        <v>72</v>
-      </c>
-      <c r="F102" s="1">
+      <c r="F102" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2041</v>
       </c>
-      <c r="G102" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>Event 72</v>
-      </c>
+      <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2042</v>
       </c>
       <c r="D103" t="s">
-        <v>73</v>
-      </c>
-      <c r="F103" s="1">
+        <v>54</v>
+      </c>
+      <c r="E103">
+        <v>100</v>
+      </c>
+      <c r="F103" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2042</v>
       </c>
@@ -5854,9 +6633,12 @@
         <v>2043</v>
       </c>
       <c r="D104" t="s">
-        <v>74</v>
-      </c>
-      <c r="F104" s="1">
+        <v>55</v>
+      </c>
+      <c r="E104">
+        <v>-40</v>
+      </c>
+      <c r="F104" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2043</v>
       </c>
@@ -5870,9 +6652,12 @@
         <v>2044</v>
       </c>
       <c r="D105" t="s">
-        <v>75</v>
-      </c>
-      <c r="F105" s="1">
+        <v>56</v>
+      </c>
+      <c r="E105">
+        <v>100</v>
+      </c>
+      <c r="F105" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2044</v>
       </c>
@@ -5886,9 +6671,12 @@
         <v>2045</v>
       </c>
       <c r="D106" t="s">
-        <v>76</v>
-      </c>
-      <c r="F106" s="1">
+        <v>57</v>
+      </c>
+      <c r="E106">
+        <v>75</v>
+      </c>
+      <c r="F106" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2045</v>
       </c>
@@ -5902,9 +6690,12 @@
         <v>2046</v>
       </c>
       <c r="D107" t="s">
-        <v>77</v>
-      </c>
-      <c r="F107" s="1">
+        <v>58</v>
+      </c>
+      <c r="E107">
+        <v>50</v>
+      </c>
+      <c r="F107" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2046</v>
       </c>
@@ -5917,42 +6708,33 @@
       <c r="A108">
         <v>2047</v>
       </c>
-      <c r="D108" t="s">
-        <v>78</v>
-      </c>
-      <c r="F108" s="1">
+      <c r="F108" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2047</v>
       </c>
-      <c r="G108" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>Event 78</v>
-      </c>
+      <c r="G108" s="1"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2048</v>
       </c>
-      <c r="D109" t="s">
-        <v>79</v>
-      </c>
-      <c r="F109" s="1">
+      <c r="F109" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2048</v>
       </c>
-      <c r="G109" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>Event 79</v>
-      </c>
+      <c r="G109" s="1"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2049</v>
       </c>
       <c r="D110" t="s">
-        <v>80</v>
-      </c>
-      <c r="F110" s="1">
+        <v>59</v>
+      </c>
+      <c r="E110">
+        <v>100</v>
+      </c>
+      <c r="F110" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2049</v>
       </c>
@@ -5966,15 +6748,18 @@
         <v>2050</v>
       </c>
       <c r="D111" t="s">
-        <v>81</v>
-      </c>
-      <c r="F111" s="1">
+        <v>102</v>
+      </c>
+      <c r="E111">
+        <v>-40</v>
+      </c>
+      <c r="F111" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2050</v>
       </c>
       <c r="G111" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Event 81</v>
+        <v>Projected Populaton 379,419,102</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -5982,9 +6767,12 @@
         <v>2051</v>
       </c>
       <c r="D112" t="s">
-        <v>82</v>
-      </c>
-      <c r="F112" s="1">
+        <v>60</v>
+      </c>
+      <c r="E112">
+        <v>100</v>
+      </c>
+      <c r="F112" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2051</v>
       </c>
@@ -5998,9 +6786,12 @@
         <v>2052</v>
       </c>
       <c r="D113" t="s">
-        <v>83</v>
-      </c>
-      <c r="F113" s="1">
+        <v>61</v>
+      </c>
+      <c r="E113">
+        <v>75</v>
+      </c>
+      <c r="F113" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2052</v>
       </c>
@@ -6014,9 +6805,12 @@
         <v>2051</v>
       </c>
       <c r="D114" t="s">
-        <v>84</v>
-      </c>
-      <c r="F114" s="1">
+        <v>62</v>
+      </c>
+      <c r="E114">
+        <v>50</v>
+      </c>
+      <c r="F114" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2051</v>
       </c>
@@ -6030,9 +6824,12 @@
         <v>2052</v>
       </c>
       <c r="D115" t="s">
-        <v>85</v>
-      </c>
-      <c r="F115" s="1">
+        <v>63</v>
+      </c>
+      <c r="E115">
+        <v>-100</v>
+      </c>
+      <c r="F115" s="13">
         <f t="shared" ca="1" si="2"/>
         <v>2052</v>
       </c>
@@ -6064,12 +6861,12 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -6077,22 +6874,22 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -6100,22 +6897,22 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>1982</v>
@@ -6123,7 +6920,7 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="C16">
         <v>1994</v>
@@ -6131,7 +6928,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C17">
         <v>2015</v>
@@ -6139,44 +6936,44 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="C19">
         <v>1987</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C22">
         <v>2021</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>2022</v>
@@ -6199,17 +6996,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -6217,7 +7014,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
power point for internal demo
</commit_message>
<xml_diff>
--- a/Timeline_ template.xlsx
+++ b/Timeline_ template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annru\Documents\capstone_annrumsey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A7D06B-53F6-4CC0-9B55-CD8931A19D10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A7DFF0-BADA-49E5-9D3F-B56B52C8E7BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3E5591EE-1479-4915-B308-C3BDB3157271}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Year</t>
   </si>
@@ -443,6 +443,12 @@
   </si>
   <si>
     <t>Projected Populaton 379,419,102</t>
+  </si>
+  <si>
+    <t>1994 First GMO Plant Tomato</t>
+  </si>
+  <si>
+    <t>2021 CRISPR potential for COVID-19</t>
   </si>
 </sst>
 </file>
@@ -665,7 +671,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1D79CFC-0669-4DFE-BB2D-516CDBB97E4E}" type="CELLRANGE">
+                    <a:fld id="{ED6E639E-D41B-486F-9703-5064AA2B73A4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -699,7 +705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD76F921-E6D2-4250-B477-3F7937E0589E}" type="CELLRANGE">
+                    <a:fld id="{3FF0B323-9A23-49F1-9F42-D38059F74F70}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -733,7 +739,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CF2D628-A0FA-4DFA-9818-707DE5FB485F}" type="CELLRANGE">
+                    <a:fld id="{A9F03CF7-B6C4-401D-B4B4-92A3178CCE9E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -767,7 +773,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31131255-B828-4966-829D-43E13058975F}" type="CELLRANGE">
+                    <a:fld id="{57F0E5E9-AF69-431B-BF86-A7B193EC7BFD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -801,7 +807,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D5CE357C-90CC-47EA-BFB0-2314B882F225}" type="CELLRANGE">
+                    <a:fld id="{58B99D1D-62A2-41D7-AE4D-6B49D699E0BA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -835,7 +841,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42BE8F11-2492-4C22-A2A6-740B61B53A2A}" type="CELLRANGE">
+                    <a:fld id="{260A3697-5E28-4CAE-A36E-558F417D8002}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -869,7 +875,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8D9AAF3-C7EA-4338-889C-E438DE6D7340}" type="CELLRANGE">
+                    <a:fld id="{D37EB81C-C47E-46E1-9326-E5BB9FA6DB04}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -903,7 +909,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB1D9E25-F548-4011-BDFE-5D4D863B9D4A}" type="CELLRANGE">
+                    <a:fld id="{CB457A6D-640B-4E81-85C7-7C739ECB1597}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -937,7 +943,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02CA3E5F-680F-49E2-9B72-6118C7A113F8}" type="CELLRANGE">
+                    <a:fld id="{F7F3E790-51FB-4C8A-9C86-25EE371D0456}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -971,7 +977,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F740033C-2EC3-4F92-A2DE-556915799DD9}" type="CELLRANGE">
+                    <a:fld id="{3293C700-708A-4025-A7CE-2C256611AFFC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1005,7 +1011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{17980427-A89E-4BE5-A0B4-D4EF1444DAFB}" type="CELLRANGE">
+                    <a:fld id="{A867111F-75D7-491A-8F0F-D4501068C937}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1039,7 +1045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1344C3FD-56C0-43D5-93C5-8086A65FFF1D}" type="CELLRANGE">
+                    <a:fld id="{DB5A01B6-5220-4030-950D-7191FF5D3610}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1073,7 +1079,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2892ECD1-787B-4444-945C-1899457696D5}" type="CELLRANGE">
+                    <a:fld id="{D0879E36-94F3-44F6-A217-CBA2336C8ABE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1107,7 +1113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE576867-0CA2-4DFE-9EA5-8F11D8FC1CC6}" type="CELLRANGE">
+                    <a:fld id="{6BED09F4-7F36-40CF-81E0-989A37A1AD9A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1141,7 +1147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E357F714-BE2F-45AC-98FD-BECC071E7697}" type="CELLRANGE">
+                    <a:fld id="{C08B0F6E-A010-4842-9229-8AFE937B43FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1175,7 +1181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC041094-250E-4B14-9D9B-5606A67D5E6A}" type="CELLRANGE">
+                    <a:fld id="{8DC6C074-F543-4E0D-BE2F-26CBE24328E7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1209,7 +1215,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{670A4DFB-C865-40FB-BC58-7A43D1FD8B8A}" type="CELLRANGE">
+                    <a:fld id="{3A1034FF-0F27-4537-A761-8F47CE73E8AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1243,7 +1249,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D538846C-9F37-4393-A4FF-2E1B9076EA1B}" type="CELLRANGE">
+                    <a:fld id="{886DA293-96B9-4884-95C2-90C4BD6BA388}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1277,7 +1283,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE3CA1D7-DFEC-4B3F-AD50-F5BB71459ADF}" type="CELLRANGE">
+                    <a:fld id="{E699C004-0A6B-4680-9A1A-514F8D59F7AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1311,7 +1317,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5A67C7B-6847-4C85-B9A2-9A3E2ACDB8DB}" type="CELLRANGE">
+                    <a:fld id="{2CFB8959-62CA-49CA-B1BC-16F47F05D14B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1345,7 +1351,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2ED4214-4931-45FC-AC95-D9893F86EC47}" type="CELLRANGE">
+                    <a:fld id="{099FE743-76A7-4C4C-B3B1-5048468D1DB6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1379,7 +1385,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BB4E271D-0502-48AA-8252-3774E28B9C0A}" type="CELLRANGE">
+                    <a:fld id="{C7669CCF-D6A8-4B59-85FC-430BB08D1EFB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1413,7 +1419,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B1509BF-5E13-4399-B97B-1D499C34EC72}" type="CELLRANGE">
+                    <a:fld id="{60212ED7-9882-49D7-BD32-C7F8E36C403B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1447,7 +1453,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A51FAF1-EE03-4E62-BB90-1C722CE08397}" type="CELLRANGE">
+                    <a:fld id="{5BAFB109-ABE3-4F14-8A4E-F6F3EB8D6E34}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1481,7 +1487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32858929-74C6-45E4-A83C-DF89C12A922B}" type="CELLRANGE">
+                    <a:fld id="{31CAB08F-ED83-49F1-9F0C-BC6B24604724}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1515,7 +1521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCB795AC-04F8-47E6-87B4-AD56E33A8B32}" type="CELLRANGE">
+                    <a:fld id="{EB77A806-CE06-4F00-92D9-0A6140E51B3B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1549,7 +1555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9665B5D7-FC16-4B9A-BAFC-C8DCE16F3883}" type="CELLRANGE">
+                    <a:fld id="{EA400944-E316-4829-A69A-C2D9C979D0CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1583,7 +1589,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{095D6273-334F-4E6F-91F1-F93015757A33}" type="CELLRANGE">
+                    <a:fld id="{A8A082DD-0EEF-4ACC-AC81-79F92E7A6E8A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1617,7 +1623,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB7A2EF4-9093-48FC-8F3B-8324232F9468}" type="CELLRANGE">
+                    <a:fld id="{37BDC1BB-1EB6-4D6D-A11A-F367892F5225}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1651,7 +1657,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D753F2E-29D2-4556-AFAB-A6A6507D7B39}" type="CELLRANGE">
+                    <a:fld id="{A25A442C-02C2-4D1C-8F24-3599F692AA3C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1685,7 +1691,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AAEEE67-C6FA-4D2E-B3E7-A3307964E534}" type="CELLRANGE">
+                    <a:fld id="{2583AC80-0B4B-4791-AEE0-95956A8527F1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1719,7 +1725,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C16D6DC4-2443-4AD9-83DB-F4A1D917F896}" type="CELLRANGE">
+                    <a:fld id="{9581DCBD-795D-45D9-9FD8-1ADC23CF0DD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1753,7 +1759,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B51A53A3-44E0-437D-9D0E-D3D674A61822}" type="CELLRANGE">
+                    <a:fld id="{D54A8732-C7E4-492D-A3FA-27CFCB46F4F4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1787,7 +1793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9D5A124A-8914-43FB-8229-A82B38348B52}" type="CELLRANGE">
+                    <a:fld id="{3DC8DF71-8E70-4BCF-932B-16E5504F147D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1821,7 +1827,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9E2CA3A4-5CF5-4D61-B33E-3386F63E29EF}" type="CELLRANGE">
+                    <a:fld id="{CE39A347-48BE-4667-9F55-29476C4A2345}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1855,7 +1861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE001725-27F1-489D-AC24-D427BCD6B031}" type="CELLRANGE">
+                    <a:fld id="{14AF1350-1B9C-458D-BDA3-805594C774EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1889,7 +1895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{460486E2-C104-4B00-89C6-CC4427ACF439}" type="CELLRANGE">
+                    <a:fld id="{A8F75A78-4346-4D9C-A864-0CD6C4A5E0F5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1923,7 +1929,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38C3396B-78CC-43F7-8B53-98E6AFD34F4A}" type="CELLRANGE">
+                    <a:fld id="{3E00DB97-3D25-482F-9CD4-A643FF9D8634}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1957,7 +1963,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67FDEA87-F05C-45FB-A7B9-C117BDBA18DF}" type="CELLRANGE">
+                    <a:fld id="{C57909F2-F91F-463F-AD73-909D6CBC945F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1991,7 +1997,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{217258DE-37EF-45E9-AD07-5E751CA122DF}" type="CELLRANGE">
+                    <a:fld id="{3246EF99-F42B-4AAD-9A5F-09CA8E613A18}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2025,7 +2031,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70C36138-6EEE-4845-86C1-3F53A765F9C8}" type="CELLRANGE">
+                    <a:fld id="{E105197D-9F82-461C-9D83-B60DD8E8F4F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2059,7 +2065,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23313194-F89C-4C28-A670-2F65B9F6C08F}" type="CELLRANGE">
+                    <a:fld id="{99F4441A-EC33-499D-9864-9C30A1E2AA8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2093,7 +2099,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66B8A288-E5A9-4BD9-AD54-4A182DD9A89E}" type="CELLRANGE">
+                    <a:fld id="{C80EC91B-1DDC-4F1C-AAA9-995BEF57DC3F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2127,7 +2133,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{55C15F8E-B686-4670-84A9-C16888462780}" type="CELLRANGE">
+                    <a:fld id="{014E03DF-F170-4D82-ACE6-0FA12C972747}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2161,7 +2167,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{67121C33-48C0-416C-A1B4-4B2AEC9E3DB1}" type="CELLRANGE">
+                    <a:fld id="{ED555117-4425-4735-9E41-B3BB0BFDB5B9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2195,7 +2201,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2730DD7B-F2A6-42AB-A247-9E698E59439F}" type="CELLRANGE">
+                    <a:fld id="{D9CE3AB1-1963-4EBA-897B-78FDB5BCAA30}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2229,7 +2235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2FCE6931-B219-4BFB-9399-F9E7AE9216B5}" type="CELLRANGE">
+                    <a:fld id="{EDB549B7-25A9-4545-80D9-1B120C365CBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2263,7 +2269,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E721266-8427-42EC-9867-49DB8D06235C}" type="CELLRANGE">
+                    <a:fld id="{83E54EA0-803C-43C3-BBBF-B0CC63F1DE61}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2297,7 +2303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9429563C-0556-4D83-BF19-72BC8E6CB923}" type="CELLRANGE">
+                    <a:fld id="{0C3CBF99-2CF6-40F3-A637-2B219962D8D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2331,7 +2337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{129E86EA-7E84-4E51-B00E-CD77A7D6E3B2}" type="CELLRANGE">
+                    <a:fld id="{6C716D01-9ADB-4AB2-9A76-0D0D0EF7715B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2365,7 +2371,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE854FCA-7568-4751-8589-0ED8FFB32446}" type="CELLRANGE">
+                    <a:fld id="{472B3B83-B8CB-4AE7-A973-B99E8A004461}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2399,7 +2405,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{863363AB-F191-4CEA-987F-D6E82089E96F}" type="CELLRANGE">
+                    <a:fld id="{736E97AC-3600-41C1-BFAD-26CF2F5CD950}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2433,7 +2439,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5FF9B458-CD5F-4B73-8227-779316B17064}" type="CELLRANGE">
+                    <a:fld id="{339EC48F-2283-46C8-8737-CFAE3947D00F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2467,7 +2473,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5C3EDFB-FD00-4799-92D6-8CD77EC943AE}" type="CELLRANGE">
+                    <a:fld id="{C30F40C7-6465-40A4-A7BE-5A67A7E597D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2529,7 +2535,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AA27308-D31D-427F-8C65-8527E2905210}" type="CELLRANGE">
+                    <a:fld id="{5A12D658-7BA2-44C6-A446-CBBBD8D5460A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2675,7 +2681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15ED807C-5F9C-49D3-A749-CF43F396F9F4}" type="CELLRANGE">
+                    <a:fld id="{AA981350-A5B8-4682-9CDB-81345CCBEA67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2709,7 +2715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65E2B009-20D8-4FF7-A2D5-080A3A1F9AD4}" type="CELLRANGE">
+                    <a:fld id="{CF658EA2-21B5-418F-A120-7825C1DC17F3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2743,7 +2749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B609C81-44DC-4105-9E33-614EA3249B6B}" type="CELLRANGE">
+                    <a:fld id="{C47A6FAF-6A2A-4256-A44A-929B26647195}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2861,7 +2867,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BD2290E0-0C6F-4E3A-BCF8-AF6451B413F1}" type="CELLRANGE">
+                    <a:fld id="{F9D875F4-185D-465E-85FB-60CA76756CBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2923,7 +2929,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA5398A9-009B-4E25-AC5F-6AB0D3E832C1}" type="CELLRANGE">
+                    <a:fld id="{2681779B-2BDE-4AE7-AB73-62F44B623F8C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2957,7 +2963,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C402ECC9-60CE-417F-9429-87946E6C7625}" type="CELLRANGE">
+                    <a:fld id="{BC6C152B-229D-4E4C-8E60-CF6C333B1905}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2991,7 +2997,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4C5DC74E-F565-4D69-A098-082855385829}" type="CELLRANGE">
+                    <a:fld id="{0DFA73E5-D811-4753-AC23-5B457CFD11AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3053,7 +3059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D11F772-762E-41B9-85CC-E3F6BED1C955}" type="CELLRANGE">
+                    <a:fld id="{6EFF048F-EDC1-402D-897E-79767ECF9FAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3087,7 +3093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53F7FA00-E88C-4FC7-A785-AEAC35B105A0}" type="CELLRANGE">
+                    <a:fld id="{9B6849A1-914A-4859-8983-6C45FDD36193}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3121,7 +3127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{068CF5CC-7277-4007-B2A2-32FC544714BD}" type="CELLRANGE">
+                    <a:fld id="{8FF21A58-E50B-4433-ABDB-31D92FD97702}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3155,7 +3161,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F702B9E-FB5C-4C38-A258-31FFEAE92628}" type="CELLRANGE">
+                    <a:fld id="{54A0E9B4-BE84-4EFE-A77B-37A7E51012FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3189,7 +3195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88B5C58E-37FE-4F1E-941F-AF3A7E4EBDC0}" type="CELLRANGE">
+                    <a:fld id="{87710664-E753-4B3C-9D91-521CC388C16E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3279,7 +3285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90C4F0E3-FB45-450C-B0D7-847542C85CBD}" type="CELLRANGE">
+                    <a:fld id="{4F4AAED1-893B-4AB9-986E-B93B7E4695E3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3313,7 +3319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C664A6EA-C256-4884-813F-55C3203788CE}" type="CELLRANGE">
+                    <a:fld id="{CB7ABA43-1DF7-4376-B0EA-9FBAEA6982C2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3347,7 +3353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22246D76-EC58-4764-8C74-4FD7B1395B3D}" type="CELLRANGE">
+                    <a:fld id="{138849A8-AE72-4D99-9705-F9F551691BDC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3381,7 +3387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB9E284B-EA70-44B0-A22D-4C72CE6BC559}" type="CELLRANGE">
+                    <a:fld id="{B17A2EED-3E8D-4B83-AB0C-37E6761F2CE0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4073,7 +4079,7 @@
                     <c:v>Event 24</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>First GMO Plant Tomato</c:v>
+                    <c:v>1994 First GMO Plant Tomato</c:v>
                   </c:pt>
                   <c:pt idx="25">
                     <c:v>Event 26</c:v>
@@ -4154,7 +4160,7 @@
                     <c:v>Projected Populaton 331,002,651</c:v>
                   </c:pt>
                   <c:pt idx="51">
-                    <c:v>CRISPR potential for COVID-19</c:v>
+                    <c:v>2021 CRISPR potential for COVID-19</c:v>
                   </c:pt>
                   <c:pt idx="52">
                     <c:v>2022 Bioengineered Food labels</c:v>
@@ -5281,8 +5287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3934960F-9A65-4C58-B757-BC73979C20A9}">
   <dimension ref="A30:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79:E79"/>
+    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5355,7 +5361,7 @@
         <v>1971</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f t="shared" ref="G32:G95" ca="1" si="1">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
+        <f t="shared" ref="G32:G93" ca="1" si="1">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
         <v>Event 2</v>
       </c>
     </row>
@@ -5782,7 +5788,7 @@
         <v>1994</v>
       </c>
       <c r="D55" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E55">
         <v>75</v>
@@ -5793,7 +5799,7 @@
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>First GMO Plant Tomato</v>
+        <v>1994 First GMO Plant Tomato</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -6302,7 +6308,7 @@
         <v>2021</v>
       </c>
       <c r="D82" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="E82">
         <v>-75</v>
@@ -6313,7 +6319,7 @@
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>CRISPR potential for COVID-19</v>
+        <v>2021 CRISPR potential for COVID-19</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6528,7 +6534,7 @@
         <v>2036</v>
       </c>
       <c r="G97" s="1" t="str">
-        <f t="shared" ref="G96:G115" ca="1" si="3">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
+        <f t="shared" ref="G97:G115" ca="1" si="3">OFFSET($D$30,ROW()-ROW($G$30),0,1,1)</f>
         <v>Event 67</v>
       </c>
     </row>

</xml_diff>